<commit_message>
regression update for acil acil
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="137">
   <si>
     <t>Sayı</t>
   </si>
@@ -421,6 +421,21 @@
   </si>
   <si>
     <t>Kullanıcı " Üye olmak için Bireysel Üyelik Sözleşmesi ve Ekleri'ni kabul etmeniz gerekmektedir" uyarısı ile karşılaşmalıdır.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acil Acil </t>
+  </si>
+  <si>
+    <t>Acil Acil sayfasında ;Filtreleme kısmında "Seçtikçe Getir" Seçeneğinin işaretlenerek Filtreleme Yapılması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" seçilir.     2- "Acil Acil" Sayfasında Filtreleme bölümünün en altında "Seçtikçe Sonuç Getir" seçeneği işaretlenir.                         3- Filtreleme Seçeneklerinden  " İL" seçeneği değiştirilmeye çalışılır.</t>
+  </si>
+  <si>
+    <t>Filtreleme Bölümünde "Seçtikçe Sonuç Getir" Seçeneği işaretlenmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Seçtikçe Sonuç Getir" Seçeneğini işaretleyip Filtreleme seçeneklerini seçtiğinde seçilen sonuç ekrana getirilmelidir.</t>
   </si>
 </sst>
 </file>
@@ -6891,9 +6906,9 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7362,16 +7377,30 @@
       <c r="A14" s="45">
         <v>13</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="19"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="19"/>
+      <c r="B14" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>136</v>
+      </c>
       <c r="I14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="30"/>
+      <c r="J14" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:23" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
regression update for acil acil (fault)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="555" windowWidth="16860" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="510" yWindow="555" windowWidth="16860" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Üyelik Gerektiren İşlemler" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="140">
   <si>
     <t>Sayı</t>
   </si>
@@ -437,12 +437,21 @@
   <si>
     <t>Kullanıcı "Seçtikçe Sonuç Getir" Seçeneğini işaretleyip Filtreleme seçeneklerini seçtiğinde seçilen sonuç ekrana getirilmelidir.</t>
   </si>
+  <si>
+    <t>Seçtikçe Sonuç Getir Fonksiyonu Düzgün Çalışmıyor</t>
+  </si>
+  <si>
+    <t>Uygulamanın Filtreleme Alanındaki "Seçtikçe Sonuç Getir" seçeneği işaretlendiğinde "İL" seçimi yapılamıyor</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6lQOzo05s54</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -519,6 +528,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -622,10 +637,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,8 +773,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6906,9 +6926,9 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11873,7 +11893,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11912,7 +11935,7 @@
         <v>95</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11926,7 +11949,7 @@
         <v>97</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11940,13 +11963,22 @@
         <v>99</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>139</v>
+      </c>
       <c r="N5" s="10" t="s">
         <v>96</v>
       </c>
@@ -14945,6 +14977,9 @@
       <formula1>$N$2:$N$6</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>

<commit_message>
regression update for acil acil (EMLAK)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="555" windowWidth="16860" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="510" yWindow="555" windowWidth="16860" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Üyelik Gerektiren İşlemler" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="166">
   <si>
     <t>Sayı</t>
   </si>
@@ -445,6 +445,84 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=6lQOzo05s54</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasına Giriş ve Sayfadaki ilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan " Acil Acil " tıklanır.  2- Sayfada bulunan ilanlardan herhangi biri tıklanır.                                                    3- İlan fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı Acil Acil sayfasına erişebilmeli ve yayınlanmış ilanları görüntüleyip fotoğraflarına ve ilan detaylarına erişebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki İlanların      "Tarih / Fiyat / Adrese göre Alfabetik" sira ile sonuçları getirmesi</t>
+  </si>
+  <si>
+    <t>Kullanıcı Acil Acil Sayfasındaki ilanları "Tarih, Fiyat ve Adresin Alfabetik sırasına göre sonuçları görüntüleyebilmeli.</t>
+  </si>
+  <si>
+    <t>Fiyatı Düşenler</t>
+  </si>
+  <si>
+    <t>Fiyatı Düşenler Sayfasına Erişim ve Sayfadaki ilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan  " Fiyatı Düşenler " tıklanır.                                                    2- Açılan sayfadaki ilanlar tıklanır ve fotoğrafları arasında geçiş yapılır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı Fiyatı düşenler sayfasını ve sayfadaki ilanları görüntüleyebilmeli. İlan fotoğrafları arasında geçiş yapabilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki Emlak Kategorisinin görüntülenmesi ve İlanların Görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki Emlak Kategorisinin ilanlarının Gelişmiş Sıralama İle Sıralanması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.    2- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               3-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    4-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    5-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   7-Adrese göre (A-Z) seçeneği tıklanır.         8-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   8-Adrese göre (A-Z) seçeneği tıklanır.         9-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Emlak" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli fotoğraflar arasında geçiş yapabilmelidir</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Emlak" sayfasındaki ilanları " Gelişmiş Sıralama " Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "Emlak" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Emlak" Kategorisindeki Filtreleme aracının "Seçtikçe Sonuç Getir" Özelliğinin Kullanımı</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "Emlak" kategorisine tıklamak ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Emlak" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Emlak" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenen Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Emlak" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
   </si>
 </sst>
 </file>
@@ -6926,9 +7004,9 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7401,128 +7479,242 @@
         <v>132</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="G14" s="30" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="I14" s="43" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:23" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="19"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="19"/>
+      <c r="A15" s="45">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>136</v>
+      </c>
       <c r="I15" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:23" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="45"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="19"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="19"/>
+      <c r="A16" s="45">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>144</v>
+      </c>
       <c r="I16" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="30"/>
+      <c r="J16" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="45"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="19"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="19"/>
+      <c r="A17" s="45">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="I17" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="30"/>
+      <c r="J17" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="45"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="19"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="19"/>
+      <c r="A18" s="45">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="I18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="30"/>
+      <c r="J18" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="45"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="19"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="19"/>
+      <c r="A19" s="45">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>158</v>
+      </c>
       <c r="I19" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="30"/>
+      <c r="J19" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="45"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="19"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="19"/>
+      <c r="A20" s="45">
+        <v>19</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>162</v>
+      </c>
       <c r="I20" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="30"/>
+      <c r="J20" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="45"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="19"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="19"/>
+      <c r="A21" s="45">
+        <v>20</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>165</v>
+      </c>
       <c r="I21" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="30"/>
+      <c r="J21" s="30" t="s">
+        <v>19</v>
+      </c>
       <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="45"/>
+      <c r="A22" s="45">
+        <v>21</v>
+      </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="23"/>
@@ -7549,20 +7741,7 @@
       <c r="J23" s="30"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="45"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="19"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="19"/>
-    </row>
+    <row r="24" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="45"/>
       <c r="B25" s="19"/>
@@ -7843,7 +8022,36 @@
       <c r="J44" s="30"/>
       <c r="K44" s="19"/>
     </row>
-    <row r="45" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="45">
+        <v>16</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I45" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K45" s="19"/>
+    </row>
     <row r="46" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8802,13 +9010,13 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G44">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G23 G25:G45">
       <formula1>$V$2:$V$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10">
       <formula1>$W$2:$W$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J44">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J23 J25:J45">
       <formula1>$W$2:$W$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -11893,7 +12101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>

</xml_diff>

<commit_message>
regression update for acil acil (Yedek Parça,Aksesuar, Donanım & Tuning)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="206">
   <si>
     <t>Sayı</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Kullanıcı "Seçtikçe Sonuç Getir" Seçeneğini işaretleyip Filtreleme seçeneklerini seçtiğinde seçilen sonuç ekrana getirilmelidir.</t>
   </si>
   <si>
-    <t>Seçtikçe Sonuç Getir Fonksiyonu Düzgün Çalışmıyor</t>
-  </si>
-  <si>
     <t>Uygulamanın Filtreleme Alanındaki "Seçtikçe Sonuç Getir" seçeneği işaretlendiğinde "İL" seçimi yapılamıyor</t>
   </si>
   <si>
@@ -495,9 +492,6 @@
     <t>Kullanıcı "Emlak" sayfasındaki ilanları " Gelişmiş Sıralama " Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
   </si>
   <si>
-    <t>Acil Acil Sayfasındaki Filtreleme aracının Kullanımı</t>
-  </si>
-  <si>
     <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
   </si>
   <si>
@@ -510,26 +504,152 @@
     <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
   </si>
   <si>
-    <t>"Acil Acil" sayfasındaki Kategorilerden "Emlak" kategorisine tıklamak ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
-  </si>
-  <si>
     <t>Kullanıcı "Emlak" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
   </si>
   <si>
-    <t>Acil Acil sayfası "Emlak" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenen Seçekler dahilinde değiştirmek</t>
-  </si>
-  <si>
     <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Emlak" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
   </si>
   <si>
     <t>Kullanıcı "Emlak" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Emlak" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>Acil Acil (EMLAK)</t>
+  </si>
+  <si>
+    <t>Acil Acil (VASITA)</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "Vasıta" Kategorisinin görüntülenmesi ve Sayfadaki iilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "Vasıta" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Vasıta" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli ilan fotoğrafları arasında geçiş yapabilmelidir ve İlan Detaylarını sorunsuz bir şekilde Görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki "Vasıta" Kategorisinin ilanlarının Gelişmiş Sıralama İle Sıralanması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Vasıta" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   8-Adrese göre (A-Z) seçeneği tıklanır.         9-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Vasıta" sayfasındaki ilanları " Gelişmiş Sıralama " Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "Emlak" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "Vasıta" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Vasıta" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "Vasıta" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Vasıta" Kategorisindeki Filtreleme aracının "Seçtikçe Sonuç Getir" Özelliğinin Kullanımı</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Vasıta" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "Emlak" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "Vasıta" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Vasıta" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Vasıta" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Vasıta" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Vasıta" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil (Yedek Parça, Aksesuar, Donanım &amp; Tuning )</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisinin görüntülenmesi ve Sayfadaki iilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli ilan fotoğrafları arasında geçiş yapabilmelidir ve İlan Detaylarını sorunsuz bir şekilde Görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisinin ilanlarının Gelişmiş Sıralama İle Sıralanması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   8-Adrese göre (A-Z) seçeneği tıklanır.         9-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Yedek Parça, Aksesuar, Donanım &amp; Tuning" sayfasındaki ilanları " Gelişmiş Sıralama " Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki Filtreleme aracının "Seçtikçe Sonuç Getir" Özelliğinin Kullanımı</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil (İkinci El ve Sıfır Alışveriş)</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "İkinci El ve Sıfır Alışveriş" Kategorisinin görüntülenmesi ve Sayfadaki iilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "İkinci El ve Sıfır Alışveriş" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli ilan fotoğrafları arasında geçiş yapabilmelidir ve İlan Detaylarını sorunsuz bir şekilde Görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "Yedek Parça, Aksesuar, Donanım &amp; Tuning" Kategorisi içerisinde "Seçtikçe Sonuç Getir" Filtreleme Özelliği Düzgün Çalışmıyor</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "Seçtikçe Sonuç Getir" Fonksiyonu Düzgün Çalışmıyor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -613,8 +733,41 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,6 +778,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9CC2E5"/>
         <bgColor rgb="FF9CC2E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -715,11 +878,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -854,9 +1019,29 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="İyi" xfId="2" builtinId="26"/>
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
+    <cellStyle name="Kötü" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7005,8 +7190,8 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7096,7 +7281,7 @@
       <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="49" t="s">
         <v>19</v>
       </c>
       <c r="V2" s="10" t="s">
@@ -7133,7 +7318,7 @@
       <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="6"/>
@@ -7170,7 +7355,7 @@
       <c r="I4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="6"/>
@@ -7207,7 +7392,7 @@
       <c r="I5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="6"/>
@@ -7241,7 +7426,7 @@
       <c r="I6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -7277,7 +7462,7 @@
       <c r="I7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K7" s="6"/>
@@ -7307,7 +7492,7 @@
       <c r="H8" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="6"/>
@@ -7341,7 +7526,7 @@
       <c r="I9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="48" t="s">
         <v>21</v>
       </c>
       <c r="K9" s="6"/>
@@ -7371,7 +7556,7 @@
       <c r="I10" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="49" t="s">
         <v>19</v>
       </c>
       <c r="W10" s="10" t="s">
@@ -7405,7 +7590,7 @@
       <c r="I11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="6"/>
@@ -7437,7 +7622,7 @@
       <c r="I12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="6"/>
@@ -7467,7 +7652,7 @@
       <c r="I13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="49" t="s">
         <v>19</v>
       </c>
     </row>
@@ -7479,10 +7664,10 @@
         <v>132</v>
       </c>
       <c r="C14" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>140</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>141</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>61</v>
@@ -7491,12 +7676,12 @@
         <v>16</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K14" s="19"/>
@@ -7526,7 +7711,7 @@
       <c r="I15" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="48" t="s">
         <v>21</v>
       </c>
       <c r="K15" s="19"/>
@@ -7539,10 +7724,10 @@
         <v>132</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>121</v>
@@ -7551,12 +7736,12 @@
         <v>20</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I16" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="30" t="s">
+      <c r="J16" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="19"/>
@@ -7565,14 +7750,14 @@
       <c r="A17" s="45">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>132</v>
+      <c r="B17" s="44" t="s">
+        <v>163</v>
       </c>
       <c r="C17" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>149</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>150</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>121</v>
@@ -7580,13 +7765,13 @@
       <c r="G17" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>154</v>
+      <c r="H17" s="44" t="s">
+        <v>153</v>
       </c>
       <c r="I17" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K17" s="19"/>
@@ -7595,14 +7780,14 @@
       <c r="A18" s="45">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>132</v>
+      <c r="B18" s="44" t="s">
+        <v>163</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D18" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>121</v>
@@ -7611,12 +7796,12 @@
         <v>20</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I18" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="30" t="s">
+      <c r="J18" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K18" s="19"/>
@@ -7625,14 +7810,14 @@
       <c r="A19" s="45">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>132</v>
+      <c r="B19" s="44" t="s">
+        <v>163</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D19" s="46" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E19" s="44" t="s">
         <v>121</v>
@@ -7641,12 +7826,12 @@
         <v>16</v>
       </c>
       <c r="H19" s="44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I19" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="30" t="s">
+      <c r="J19" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K19" s="19"/>
@@ -7656,27 +7841,27 @@
         <v>19</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="G20" s="30" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="44" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I20" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K20" s="19"/>
@@ -7686,13 +7871,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E21" s="44" t="s">
         <v>121</v>
@@ -7701,12 +7886,12 @@
         <v>16</v>
       </c>
       <c r="H21" s="44" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I21" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="49" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="19"/>
@@ -7715,143 +7900,329 @@
       <c r="A22" s="45">
         <v>21</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="19"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>167</v>
+      </c>
       <c r="I22" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="30"/>
+      <c r="J22" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="45"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="19"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="19"/>
+      <c r="A23" s="45">
+        <v>22</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="44" t="s">
+        <v>170</v>
+      </c>
       <c r="I23" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="30"/>
+      <c r="J23" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="45">
+        <v>23</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="I24" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="25" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="45"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="19"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="19"/>
+      <c r="A25" s="45">
+        <v>24</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="44" t="s">
+        <v>179</v>
+      </c>
       <c r="I25" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="30"/>
+      <c r="J25" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="45"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="19"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="19"/>
+      <c r="A26" s="45">
+        <v>25</v>
+      </c>
+      <c r="B26" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>182</v>
+      </c>
       <c r="I26" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="30"/>
+      <c r="J26" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="45"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="19"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="19"/>
+      <c r="A27" s="45">
+        <v>26</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>186</v>
+      </c>
       <c r="I27" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="30"/>
+      <c r="J27" s="50" t="s">
+        <v>19</v>
+      </c>
       <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="45"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="19"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="19"/>
+      <c r="A28" s="45">
+        <v>27</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="44" t="s">
+        <v>189</v>
+      </c>
       <c r="I28" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="30"/>
+      <c r="J28" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="45"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="19"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="19"/>
+      <c r="A29" s="45">
+        <v>28</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="44" t="s">
+        <v>192</v>
+      </c>
       <c r="I29" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="30"/>
+      <c r="J29" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K29" s="19"/>
     </row>
     <row r="30" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="45"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="19"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="19"/>
+      <c r="A30" s="45">
+        <v>29</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="44" t="s">
+        <v>196</v>
+      </c>
       <c r="I30" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="30"/>
+      <c r="J30" s="48" t="s">
+        <v>21</v>
+      </c>
       <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="45"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="19"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="19"/>
+      <c r="A31" s="45">
+        <v>30</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="44" t="s">
+        <v>199</v>
+      </c>
       <c r="I31" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="30"/>
+      <c r="J31" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="45"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="19"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="19"/>
+      <c r="A32" s="45">
+        <v>31</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="44" t="s">
+        <v>203</v>
+      </c>
       <c r="I32" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="30"/>
+      <c r="J32" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -8027,13 +8398,13 @@
         <v>16</v>
       </c>
       <c r="B45" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="23" t="s">
         <v>146</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>147</v>
       </c>
       <c r="E45" s="19" t="s">
         <v>121</v>
@@ -8042,7 +8413,7 @@
         <v>16</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I45" s="43" t="s">
         <v>18</v>
@@ -9010,13 +9381,13 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G23 G25:G45">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G45">
       <formula1>$V$2:$V$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10">
       <formula1>$W$2:$W$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J23 J25:J45">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J45">
       <formula1>$W$2:$W$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -12103,7 +12474,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12175,24 +12546,32 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>137</v>
+      <c r="A5" s="40" t="s">
+        <v>205</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="47" t="s">
         <v>138</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>139</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37"/>
+    <row r="6" spans="1:14" ht="183.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>137</v>
+      </c>
       <c r="N6" s="10" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
regression update for acil acil (İkinci El ve Sıfır Alışveriş)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="220">
   <si>
     <t>Sayı</t>
   </si>
@@ -643,6 +643,48 @@
   </si>
   <si>
     <t>Acil Acil Sayfasında "Seçtikçe Sonuç Getir" Fonksiyonu Düzgün Çalışmıyor</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki "İkinci El ve Sıfır Alışveriş" Kategorisinin ilanlarının Gelişmiş Sıralama İle Sıralanması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İkinci El ve Sıfır Alışveriş" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   8-Adrese göre (A-Z) seçeneği tıklanır.         9-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" sayfasındaki ilanları "Gelişmiş Sıralama" Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "İkinci El ve Sıfır Alışveriş" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İkinci El ve Sıfır Alışveriş" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "İkinci El ve Sıfır Alışveriş" Kategorisindeki Filtreleme aracının "Seçtikçe Sonuç Getir" Özelliğinin Kullanımı</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İkinci El ve Sıfır Alışveriş" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "İkinci El ve Sıfır Alışveriş" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "İkinci El ve Sıfır Alışveriş" Kategorisi içerisinde "Seçtikçe Sonuç Getir" Filtreleme Özelliği Düzgün Çalışmıyor</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "İkinci El ve Sıfır Alışveriş" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İkinci El ve Sıfır Alışveriş" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
   </si>
 </sst>
 </file>
@@ -7190,8 +7232,8 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8226,63 +8268,127 @@
       <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="45"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="19"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="19"/>
+      <c r="A33" s="45">
+        <v>32</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="44" t="s">
+        <v>208</v>
+      </c>
       <c r="I33" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="30"/>
+      <c r="J33" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="45"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="19"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="19"/>
+      <c r="A34" s="45">
+        <v>33</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="D34" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="44" t="s">
+        <v>211</v>
+      </c>
       <c r="I34" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J34" s="30"/>
+      <c r="J34" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="45"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="19"/>
+      <c r="A35" s="45">
+        <v>34</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="E35" s="44" t="s">
+        <v>214</v>
+      </c>
       <c r="G35" s="30"/>
-      <c r="H35" s="19"/>
+      <c r="H35" s="44" t="s">
+        <v>215</v>
+      </c>
       <c r="I35" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="30"/>
+      <c r="J35" s="48" t="s">
+        <v>21</v>
+      </c>
       <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="45"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="19"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="19"/>
+      <c r="A36" s="45">
+        <v>35</v>
+      </c>
+      <c r="B36" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="44" t="s">
+        <v>219</v>
+      </c>
       <c r="I36" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J36" s="30"/>
+      <c r="J36" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K36" s="19"/>
     </row>
     <row r="37" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="45"/>
+      <c r="A37" s="45">
+        <v>36</v>
+      </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
       <c r="D37" s="23"/>
@@ -12473,8 +12579,8 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12576,8 +12682,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="37"/>
+    <row r="7" spans="1:14" ht="183.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="37"/>

</xml_diff>

<commit_message>
regression update for acil acil (İş Makineleri & Sanayi)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="237">
   <si>
     <t>Sayı</t>
   </si>
@@ -685,6 +685,57 @@
   </si>
   <si>
     <t>Kullanıcı "İkinci El ve Sıfır Alışveriş" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil (İş Makineleri &amp; Sanayi)</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "İş Makineleri &amp; Sanayi" Kategorisinin görüntülenmesi ve Sayfadaki iilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "İş Makineleri &amp; Sanayi" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İş Makineleri &amp; Sanayi" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli ilan fotoğrafları arasında geçiş yapabilmelidir ve İlan Detaylarını sorunsuz bir şekilde Görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İş Makineleri &amp; Sanayi" sayfasındaki ilanları "Gelişmiş Sıralama" Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İş Makineleri &amp; Sanayi" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.</t>
+  </si>
+  <si>
+    <t>Adrese göre sıralama seçeneği bulunmuyor</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "İş Makineleri &amp; Sanayi" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İş Makineleri &amp; Sanayi" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "İş Makineleri &amp; Sanayi" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İş Makineleri &amp; Sanayi" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "İş Makineleri &amp; Sanayi" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İş Makineleri &amp; Sanayi" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "İş Makineleri &amp; Sanayi" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "İş Makineleri &amp; Sanayi" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "İş Makineleri &amp; Sanayi" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "İş Makineleri &amp; Sanayi" Kategorisi içerisinde "Seçtikçe Sonuç Getir" Filtreleme Özelliği Düzgün Çalışmıyor</t>
   </si>
 </sst>
 </file>
@@ -7232,8 +7283,8 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8389,76 +8440,158 @@
       <c r="A37" s="45">
         <v>36</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="19"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="19"/>
+      <c r="B37" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="44" t="s">
+        <v>223</v>
+      </c>
       <c r="I37" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J37" s="30"/>
+      <c r="J37" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K37" s="19"/>
     </row>
     <row r="38" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="45"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="19"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="19"/>
+      <c r="A38" s="45">
+        <v>37</v>
+      </c>
+      <c r="B38" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="44" t="s">
+        <v>224</v>
+      </c>
       <c r="I38" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J38" s="30"/>
-      <c r="K38" s="19"/>
+      <c r="J38" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="K38" s="44" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="45"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="19"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="19"/>
+      <c r="A39" s="45">
+        <v>38</v>
+      </c>
+      <c r="B39" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G39" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="44" t="s">
+        <v>229</v>
+      </c>
       <c r="I39" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="30"/>
+      <c r="J39" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="45"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="19"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="19"/>
+      <c r="A40" s="45">
+        <v>39</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="D40" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="44" t="s">
+        <v>232</v>
+      </c>
       <c r="I40" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="30"/>
+      <c r="J40" s="48" t="s">
+        <v>21</v>
+      </c>
       <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="45"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="19"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="19"/>
+      <c r="A41" s="45">
+        <v>40</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="44" t="s">
+        <v>235</v>
+      </c>
       <c r="I41" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J41" s="30"/>
+      <c r="J41" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K41" s="19"/>
     </row>
     <row r="42" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="45"/>
+      <c r="A42" s="45">
+        <v>41</v>
+      </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="23"/>
@@ -12579,8 +12712,8 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12696,8 +12829,19 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="37"/>
+    <row r="8" spans="1:14" ht="183.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="37"/>

</xml_diff>

<commit_message>
regression update for acil acil (Özel Ders Verenler)
</commit_message>
<xml_diff>
--- a/sahibinden.com.xlsx
+++ b/sahibinden.com.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="254">
   <si>
     <t>Sayı</t>
   </si>
@@ -736,13 +736,64 @@
   </si>
   <si>
     <t>Acil Acil Sayfası "İş Makineleri &amp; Sanayi" Kategorisi içerisinde "Seçtikçe Sonuç Getir" Filtreleme Özelliği Düzgün Çalışmıyor</t>
+  </si>
+  <si>
+    <t>Acil Acil (Özel Ders Verenler)</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfası "Özel Ders Verenler" Kategorisinin görüntülenmesi ve Sayfadaki iilanların görüntülenmesi</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol Kısımdan  "Acil Acil" tıklanır.                     2- Sayfadaki Kategorilerden "Özel Ders Verenler" Başlığı tıklanır.                                          3- Sayfadaki ilanlar tıklanır ve ilan görüntülenir.                                             4- İlan Fotoğrafları arasında geçiş yapılır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Özel Ders Verenler" Sayfasını ve sayfada bulunan ilanları görüntüleyebilmeli ilan fotoğrafları arasında geçiş yapabilmelidir ve İlan Detaylarını sorunsuz bir şekilde Görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasındaki "Özel Ders Verenler" Kategorisinin ilanlarının Gelişmiş Sıralama İle Sıralanması</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Özel Ders Verenler" Başlığı tıklanır.                                         3- Sayfada görüntülenen ilanların sağ üst göşesinde görünüm kısmında yer alan Gelişmiş sıralama aracı tıklanır.                               4-Fiyata Göre (Önce en Yüksek) seçeneği tıklanır.                                                    5-Fiyata Göre (Önce en düşük) seçeneği tıklanır.                                                    6-Tarihe göre (Önce En Yeni) seçeneği tıklanır.                                                    7-Tarihe göre (Önce En Eski) seçeneği Tıklanır.                                                   8-Adrese göre (A-Z) seçeneği tıklanır.         9-Adrese göre (Z-A) seçeneği tıklanır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Özel Ders Verenler" sayfasındaki ilanları "Gelişmiş Sıralama" Aracı ile Tarih, Fiyat ve Adrese göre alfabetik sıralayabilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil Sayfasında "Özel Ders Verenler" Kategorisindeki Filtreleme aracının Kullanımı</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Özel Ders Verenler" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracında Seçimler yapılır ve Aracın en altında bulunan "Ara" butonu tıklanır. </t>
+  </si>
+  <si>
+    <t>Kullanıcı "Özel Ders Verenler" Kategorisindeki İlanları Filtreleme aracını Kullanarak filtrelenen sonuçları doğru şekilde görüntüleyebilmeli</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Özel Ders Verenler" Kategorisindeki Filtreleme aracının "Seçtikçe Sonuç Getir" Özelliğinin Kullanımı</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Özel Ders Verenler" Başlığı tıklanır.                                         3- Sayfanın sol tarafında bulunan Filtreleme aracı altında "Seçtikçe Sonuç Getir" Özelliği Yanındaki Kutucuk işaretlenerek aktif edilir.                                                4- Filtreleme aracında seçimler yapılır.</t>
+  </si>
+  <si>
+    <t>"Acil Acil" sayfasındaki Kategorilerden "Özel Ders Verenler" kategorisine tıklanmalı ve Filtreleme aracı altındaki "Seçtikçe Sonuç Getir" özelliği aktif edilmelidir.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Özel Ders Verenler" Kategorisindeki ilanları "Seçtikçe Sonuç Getir" Özelliğini kullanarak filtreleyebilmeli ve seçim yaptığı filtreleme sonuçlarını görüntüleyebilmelidir.</t>
+  </si>
+  <si>
+    <t>Acil Acil sayfası "Özel Ders Verenler" Kategorisindeki İlanların Sayfa numaraları arasında geçiş yapmak ve Sayfada Listelenecek Sonuç Sayısını Belirlenmiş Seçekler dahilinde değiştirmek</t>
+  </si>
+  <si>
+    <t>1- Uygulama Ana sayfasına gidilir ve Sol kısımdaki başlıklardan "Acil Acil" tıklanır.   2- Sayfadaki Kategorilerden "Özel Ders Verenler" Başlığı tıklanır                                          3- Sayfada Listelenen Sonuçları 20 ile 50 Sonuç arasında seçim yapılır.                    4- Sayfa numaralarına tıklarnır.</t>
+  </si>
+  <si>
+    <t>Kullanıcı "Özel Ders Verenler" Kategorisindeki ilanları sayfa başına 20 veya 50 sonuç arasında görüntülenecek şekilde değiştirebilmeli ve Sayfalar arasında geçiş yaparak diğer sayfaları görüntüleyebilmelidir.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -843,6 +894,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -860,7 +919,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -881,6 +940,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -971,13 +1035,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1118,24 +1183,29 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="İyi" xfId="2" builtinId="26"/>
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Kötü" xfId="3" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nötr" xfId="4" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7283,8 +7353,8 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7380,7 +7450,7 @@
       <c r="V2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W2" s="55" t="s">
         <v>19</v>
       </c>
     </row>
@@ -7418,7 +7488,7 @@
       <c r="V3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="56" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7455,11 +7525,11 @@
       <c r="V4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -7489,7 +7559,7 @@
         <v>19</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="50" t="s">
         <v>41</v>
       </c>
     </row>
@@ -8163,7 +8233,7 @@
       <c r="I27" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="51" t="s">
         <v>19</v>
       </c>
       <c r="K27" s="19"/>
@@ -8244,7 +8314,7 @@
       <c r="E30" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="G30" s="51" t="s">
+      <c r="G30" s="52" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="44" t="s">
@@ -8592,111 +8662,259 @@
       <c r="A42" s="45">
         <v>41</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="19"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="19"/>
+      <c r="B42" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C42" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>239</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="44" t="s">
+        <v>240</v>
+      </c>
       <c r="I42" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="30"/>
+      <c r="J42" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K42" s="19"/>
     </row>
     <row r="43" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="45"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="19"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="19"/>
+      <c r="A43" s="45">
+        <v>42</v>
+      </c>
+      <c r="B43" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C43" s="44" t="s">
+        <v>241</v>
+      </c>
+      <c r="D43" s="46" t="s">
+        <v>242</v>
+      </c>
+      <c r="E43" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="44" t="s">
+        <v>243</v>
+      </c>
       <c r="I43" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J43" s="30"/>
+      <c r="J43" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K43" s="19"/>
     </row>
     <row r="44" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="45"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="19"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="19"/>
+      <c r="A44" s="45">
+        <v>43</v>
+      </c>
+      <c r="B44" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="E44" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="44" t="s">
+        <v>246</v>
+      </c>
       <c r="I44" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J44" s="30"/>
+      <c r="J44" s="49" t="s">
+        <v>19</v>
+      </c>
       <c r="K44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="45">
-        <v>16</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>121</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="E45" s="44" t="s">
+        <v>249</v>
       </c>
       <c r="G45" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>147</v>
+      <c r="H45" s="44" t="s">
+        <v>250</v>
       </c>
       <c r="I45" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="J45" s="30" t="s">
+      <c r="J45" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="45">
+        <v>45</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="D46" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="E46" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="I46" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K45" s="19"/>
-    </row>
-    <row r="46" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
     <row r="47" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="45">
+        <v>16</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I52" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J52" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K52" s="19"/>
+    </row>
+    <row r="53" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="45">
+        <v>16</v>
+      </c>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="19"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" s="30"/>
+      <c r="K53" s="19"/>
+    </row>
+    <row r="54" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="45">
+        <v>16</v>
+      </c>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="19"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="30"/>
+      <c r="K59" s="19"/>
+    </row>
+    <row r="60" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="45">
+        <v>16</v>
+      </c>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="19"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="J65" s="30"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:11" ht="267.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9620,13 +9838,13 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G45">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G46 G52:G53 G59 G65">
       <formula1>$V$2:$V$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J10">
       <formula1>$W$2:$W$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J45">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J9 J11:J46 J52:J53 J59 J65">
       <formula1>$W$2:$W$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -12791,7 +13009,7 @@
       <c r="B5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="53" t="s">
         <v>137</v>
       </c>
       <c r="D5" s="47" t="s">
@@ -12808,7 +13026,7 @@
       <c r="B6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="54" t="s">
         <v>137</v>
       </c>
       <c r="N6" s="10" t="s">
@@ -12822,7 +13040,7 @@
       <c r="B7" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="54" t="s">
         <v>137</v>
       </c>
       <c r="N7" s="10" t="s">
@@ -12836,7 +13054,7 @@
       <c r="B8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>137</v>
       </c>
       <c r="N8" s="10" t="s">

</xml_diff>